<commit_message>
edit on oda karyalaya agadi dhalaan file
</commit_message>
<xml_diff>
--- a/ofc/estimates/वडा कार्यालय अगाडी ढलान/वडा कार्यालय अगाडी ढलान गरि ब्लक बिछ्याउने कार्य .xlsx
+++ b/ofc/estimates/वडा कार्यालय अगाडी ढलान/वडा कार्यालय अगाडी ढलान गरि ब्लक बिछ्याउने कार्य .xlsx
@@ -386,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -444,12 +444,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -601,6 +614,39 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,25 +657,19 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -653,32 +693,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1357,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,116 +1397,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
       <c r="O6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1532,10 +1554,10 @@
         <v>48</v>
       </c>
       <c r="C9" s="36"/>
-      <c r="D9" s="90" t="s">
+      <c r="D9" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="91"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="36"/>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
@@ -1587,11 +1609,11 @@
       <c r="C11" s="38">
         <v>1</v>
       </c>
-      <c r="D11" s="92">
+      <c r="D11" s="76">
         <f>(SQRT(((SUM(D10:F10))/2)*(((SUM(D10:F10))/2)-D10)*(((SUM(D10:F10))/2)-E10)*(((SUM(D10:F10))/2)-F10)))</f>
         <v>5.7603528014178709</v>
       </c>
-      <c r="E11" s="93" t="e">
+      <c r="E11" s="77" t="e">
         <f t="shared" ref="E11" si="0">(SQRT(((SUM(B11:D11))/2)*(((SUM(B11:D11))/2)-B11)*(((SUM(B11:D11))/2)-C11)*(((SUM(B11:D11))/2)-D11)))*A11</f>
         <v>#NUM!</v>
       </c>
@@ -1649,11 +1671,11 @@
       <c r="C13" s="38">
         <v>1</v>
       </c>
-      <c r="D13" s="92">
+      <c r="D13" s="76">
         <f>(SQRT(((SUM(D12:F12))/2)*(((SUM(D12:F12))/2)-D12)*(((SUM(D12:F12))/2)-E12)*(((SUM(D12:F12))/2)-F12)))</f>
         <v>5.370012282971941</v>
       </c>
-      <c r="E13" s="93" t="e">
+      <c r="E13" s="77" t="e">
         <f t="shared" ref="E13" si="2">(SQRT(((SUM(B13:D13))/2)*(((SUM(B13:D13))/2)-B13)*(((SUM(B13:D13))/2)-C13)*(((SUM(B13:D13))/2)-D13)))*A13</f>
         <v>#NUM!</v>
       </c>
@@ -1838,10 +1860,10 @@
         <v>42</v>
       </c>
       <c r="C19" s="19"/>
-      <c r="D19" s="90" t="s">
+      <c r="D19" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="91"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="21"/>
       <c r="G19" s="23"/>
       <c r="H19" s="22"/>
@@ -1850,15 +1872,15 @@
       <c r="K19" s="21"/>
       <c r="M19" s="25"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="71" t="s">
+      <c r="O19" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="71"/>
-      <c r="S19" s="71"/>
-      <c r="T19" s="71"/>
-      <c r="U19" s="71"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -1897,11 +1919,11 @@
       <c r="C21" s="38">
         <v>1</v>
       </c>
-      <c r="D21" s="92">
+      <c r="D21" s="76">
         <f>(SQRT(((SUM(D20:F20))/2)*(((SUM(D20:F20))/2)-D20)*(((SUM(D20:F20))/2)-E20)*(((SUM(D20:F20))/2)-F20)))</f>
         <v>5.7603528014178709</v>
       </c>
-      <c r="E21" s="93" t="e">
+      <c r="E21" s="77" t="e">
         <f t="shared" ref="E21" si="6">(SQRT(((SUM(B21:D21))/2)*(((SUM(B21:D21))/2)-B21)*(((SUM(B21:D21))/2)-C21)*(((SUM(B21:D21))/2)-D21)))*A21</f>
         <v>#NUM!</v>
       </c>
@@ -1959,11 +1981,11 @@
       <c r="C23" s="38">
         <v>1</v>
       </c>
-      <c r="D23" s="92">
+      <c r="D23" s="76">
         <f>(SQRT(((SUM(D22:F22))/2)*(((SUM(D22:F22))/2)-D22)*(((SUM(D22:F22))/2)-E22)*(((SUM(D22:F22))/2)-F22)))</f>
         <v>5.370012282971941</v>
       </c>
-      <c r="E23" s="93" t="e">
+      <c r="E23" s="77" t="e">
         <f t="shared" ref="E23" si="7">(SQRT(((SUM(B23:D23))/2)*(((SUM(B23:D23))/2)-B23)*(((SUM(B23:D23))/2)-C23)*(((SUM(B23:D23))/2)-D23)))*A23</f>
         <v>#NUM!</v>
       </c>
@@ -2118,10 +2140,10 @@
         <v>41</v>
       </c>
       <c r="C29" s="19"/>
-      <c r="D29" s="90" t="s">
+      <c r="D29" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="91"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="21"/>
       <c r="G29" s="23"/>
       <c r="H29" s="22"/>
@@ -2174,11 +2196,11 @@
       <c r="C31" s="38">
         <v>1</v>
       </c>
-      <c r="D31" s="92">
+      <c r="D31" s="76">
         <f>(SQRT(((SUM(D30:F30))/2)*(((SUM(D30:F30))/2)-D30)*(((SUM(D30:F30))/2)-E30)*(((SUM(D30:F30))/2)-F30)))</f>
         <v>5.7603528014178709</v>
       </c>
-      <c r="E31" s="93" t="e">
+      <c r="E31" s="77" t="e">
         <f t="shared" ref="E31" si="9">(SQRT(((SUM(B31:D31))/2)*(((SUM(B31:D31))/2)-B31)*(((SUM(B31:D31))/2)-C31)*(((SUM(B31:D31))/2)-D31)))*A31</f>
         <v>#NUM!</v>
       </c>
@@ -2236,11 +2258,11 @@
       <c r="C33" s="38">
         <v>1</v>
       </c>
-      <c r="D33" s="92">
+      <c r="D33" s="76">
         <f>(SQRT(((SUM(D32:F32))/2)*(((SUM(D32:F32))/2)-D32)*(((SUM(D32:F32))/2)-E32)*(((SUM(D32:F32))/2)-F32)))</f>
         <v>5.370012282971941</v>
       </c>
-      <c r="E33" s="93" t="e">
+      <c r="E33" s="77" t="e">
         <f t="shared" ref="E33" si="11">(SQRT(((SUM(B33:D33))/2)*(((SUM(B33:D33))/2)-B33)*(((SUM(B33:D33))/2)-C33)*(((SUM(B33:D33))/2)-D33)))*A33</f>
         <v>#NUM!</v>
       </c>
@@ -2398,10 +2420,10 @@
         <v>54</v>
       </c>
       <c r="C39" s="42"/>
-      <c r="D39" s="90" t="s">
+      <c r="D39" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="91"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="43"/>
       <c r="G39" s="39"/>
       <c r="H39" s="43"/>
@@ -2440,11 +2462,11 @@
       <c r="C41" s="38">
         <v>1</v>
       </c>
-      <c r="D41" s="92">
+      <c r="D41" s="76">
         <f>(SQRT(((SUM(D40:F40))/2)*(((SUM(D40:F40))/2)-D40)*(((SUM(D40:F40))/2)-E40)*(((SUM(D40:F40))/2)-F40)))</f>
         <v>5.7603528014178709</v>
       </c>
-      <c r="E41" s="93" t="e">
+      <c r="E41" s="77" t="e">
         <f t="shared" ref="E41" si="14">(SQRT(((SUM(B41:D41))/2)*(((SUM(B41:D41))/2)-B41)*(((SUM(B41:D41))/2)-C41)*(((SUM(B41:D41))/2)-D41)))*A41</f>
         <v>#NUM!</v>
       </c>
@@ -2493,11 +2515,11 @@
       <c r="C43" s="38">
         <v>1</v>
       </c>
-      <c r="D43" s="92">
+      <c r="D43" s="76">
         <f>(SQRT(((SUM(D42:F42))/2)*(((SUM(D42:F42))/2)-D42)*(((SUM(D42:F42))/2)-E42)*(((SUM(D42:F42))/2)-F42)))</f>
         <v>5.370012282971941</v>
       </c>
-      <c r="E43" s="93" t="e">
+      <c r="E43" s="77" t="e">
         <f t="shared" ref="E43" si="15">(SQRT(((SUM(B43:D43))/2)*(((SUM(B43:D43))/2)-B43)*(((SUM(B43:D43))/2)-C43)*(((SUM(B43:D43))/2)-D43)))*A43</f>
         <v>#NUM!</v>
       </c>
@@ -2722,14 +2744,12 @@
       <c r="B53" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="67">
+      <c r="C53" s="78">
         <f>J51</f>
         <v>32334.486292949798</v>
       </c>
-      <c r="D53" s="67"/>
-      <c r="E53" s="39">
-        <v>100</v>
-      </c>
+      <c r="D53" s="78"/>
+      <c r="E53" s="52"/>
       <c r="F53" s="51"/>
       <c r="G53" s="52"/>
       <c r="H53" s="51"/>
@@ -2737,16 +2757,16 @@
       <c r="J53" s="54"/>
       <c r="K53" s="55"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="56"/>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="70">
+      <c r="C54" s="95">
         <v>28000</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="39"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="96"/>
       <c r="F54" s="49"/>
       <c r="G54" s="48"/>
       <c r="H54" s="48"/>
@@ -2754,16 +2774,16 @@
       <c r="J54" s="48"/>
       <c r="K54" s="49"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="56"/>
       <c r="B55" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="70">
+      <c r="C55" s="81">
         <f>C54-C57-C58</f>
         <v>26600</v>
       </c>
-      <c r="D55" s="70"/>
+      <c r="D55" s="81"/>
       <c r="E55" s="39">
         <f>C55/C53*100</f>
         <v>82.265107783078832</v>
@@ -2775,16 +2795,16 @@
       <c r="J55" s="48"/>
       <c r="K55" s="49"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="56"/>
       <c r="B56" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="67">
+      <c r="C56" s="78">
         <f>C53-C55</f>
         <v>5734.4862929497976</v>
       </c>
-      <c r="D56" s="67"/>
+      <c r="D56" s="78"/>
       <c r="E56" s="39">
         <f>100-E55</f>
         <v>17.734892216921168</v>
@@ -2796,16 +2816,16 @@
       <c r="J56" s="48"/>
       <c r="K56" s="49"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="56"/>
       <c r="B57" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="67">
+      <c r="C57" s="78">
         <f>C54*0.03</f>
         <v>840</v>
       </c>
-      <c r="D57" s="67"/>
+      <c r="D57" s="78"/>
       <c r="E57" s="39">
         <v>3</v>
       </c>
@@ -2816,16 +2836,16 @@
       <c r="J57" s="48"/>
       <c r="K57" s="49"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="56"/>
       <c r="B58" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="67">
+      <c r="C58" s="78">
         <f>C54*0.02</f>
         <v>560</v>
       </c>
-      <c r="D58" s="67"/>
+      <c r="D58" s="78"/>
       <c r="E58" s="39">
         <v>2</v>
       </c>
@@ -2907,19 +2927,6 @@
     <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="O19:U19"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="A7:F7"/>
@@ -2935,6 +2942,19 @@
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="O19:U19"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -2971,90 +2991,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="85" t="e">
+      <c r="C6" s="82" t="e">
         <f>F39</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="86"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3062,11 +3082,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="85" t="e">
+      <c r="J6" s="82" t="e">
         <f>I39</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="86"/>
+      <c r="K6" s="83"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -3075,77 +3095,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="I7" s="81" t="s">
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="I7" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="str">
+      <c r="A8" s="70" t="str">
         <f>estimate!A6</f>
         <v xml:space="preserve">Project:- वडा कार्यालय अगाडी ढलान गरि ब्लक बिछ्याउने कार्य </v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="I8" s="82" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="I8" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="str">
+      <c r="A9" s="92" t="str">
         <f>estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="I9" s="82" t="s">
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="I9" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="78" t="s">
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="88" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3164,8 +3184,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="79"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="88"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="148.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -3897,13 +3917,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3917,6 +3930,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>